<commit_message>
benchmark 1 object af
</commit_message>
<xml_diff>
--- a/Week 5/Benchmark.xlsx
+++ b/Week 5/Benchmark.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -11,13 +11,48 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="10">
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>II</t>
+  </si>
+  <si>
+    <t>III</t>
+  </si>
+  <si>
+    <t>IV</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>1.</t>
+  </si>
+  <si>
+    <t>2.</t>
+  </si>
+  <si>
+    <t>3.</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -54,7 +89,51 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B2:E5">
+  <autoFilter ref="B2:E5"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="I" totalsRowLabel="Total"/>
+    <tableColumn id="2" name="II"/>
+    <tableColumn id="3" name="III"/>
+    <tableColumn id="4" name="IV"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table24" displayName="Table24" ref="B10:E13">
+  <autoFilter ref="B10:E13"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="I" totalsRowLabel="Total"/>
+    <tableColumn id="2" name="II"/>
+    <tableColumn id="3" name="III"/>
+    <tableColumn id="4" name="IV"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table245" displayName="Table245" ref="B18:E21">
+  <autoFilter ref="B18:E21"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="I" totalsRowLabel="Total"/>
+    <tableColumn id="2" name="II"/>
+    <tableColumn id="3" name="III"/>
+    <tableColumn id="4" name="IV"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -343,36 +422,176 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="6" width="11" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>0</v>
+      </c>
+      <c r="C18" t="s">
+        <v>1</v>
+      </c>
+      <c r="D18" t="s">
+        <v>2</v>
+      </c>
+      <c r="E18" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20">
+        <v>3462</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="3">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+  </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>